<commit_message>
one step. Not finished yet
</commit_message>
<xml_diff>
--- a/OptimalBuildingLevel.xlsx
+++ b/OptimalBuildingLevel.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="BFR" sheetId="4" r:id="rId1"/>
-    <sheet name="SAT" sheetId="3" r:id="rId2"/>
+    <sheet name="HGEC" sheetId="5" r:id="rId2"/>
+    <sheet name="SAT" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="69">
   <si>
     <t>Alphas</t>
   </si>
@@ -204,9 +205,6 @@
     <t>Flight computer</t>
   </si>
   <si>
-    <t>Ion Drive</t>
-  </si>
-  <si>
     <t>Attitude control</t>
   </si>
   <si>
@@ -228,7 +226,13 @@
     <t>Sat-HGEC</t>
   </si>
   <si>
-    <t>Ion-HGEC</t>
+    <t>Sat-Ion Drive</t>
+  </si>
+  <si>
+    <t>Sat-Ion-HGEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HGEC </t>
   </si>
 </sst>
 </file>
@@ -295,7 +299,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -446,6 +450,21 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -464,7 +483,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -519,6 +538,17 @@
     <xf numFmtId="43" fontId="0" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="5" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="5" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="5" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Millares" xfId="3" builtinId="3"/>
@@ -621,6 +651,87 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>200512</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>190574</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4962525" y="7239000"/>
+          <a:ext cx="3486637" cy="533474"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>828675</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>419460</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>66744</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4991100" y="7743825"/>
+          <a:ext cx="2581635" cy="495369"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1522,10 +1633,301 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="37"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="30"/>
+      <c r="E4" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="38"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="8"/>
+      <c r="E5" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="39"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="8"/>
+      <c r="E6" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="36"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
+      <c r="B11" s="10"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="54" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="55" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="57">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="58">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="60">
+        <f>SUMPRODUCT(B19:L19,B16:L16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="61">
+        <f>SUMPRODUCT(B18:L18,B16:L16)</f>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="21">
+        <f>B16/B17</f>
+        <v>4.7619047619047619</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="46">
+        <f>B24/$B$27</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="63">
+        <f>B25*$B$41</f>
+        <v>27240.476190476194</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="42">
+        <f>SUM(B24:L24)</f>
+        <v>4.7619047619047619</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="64">
+        <f>B25</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="6">
+        <v>780000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="44">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="25">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="41">
+        <f>B38/24/B28/B31</f>
+        <v>775084.61538461538</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="42">
+        <f>B32-B35</f>
+        <v>4915.3846153846243</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="35">
+        <f>B36-B21-B20</f>
+        <v>1315.3846153846243</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="27">
+        <f>(B32-B20-(B31*(1-B34)/170+1)*B21/(1+B33))*B31*B28*24</f>
+        <v>1897407138.4615383</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" s="43">
+        <f>((B32-B20)*(1+B33)/B21-1)*170/2/(1-B34)</f>
+        <v>27240.476190476194</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="27">
+        <f>(B32-B20-((B41*(1-B34)/170+1)*B21/(1+B33)))*B41*B28*24</f>
+        <v>253839329670.32968</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,7 +1985,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="8">
         <v>1490</v>
@@ -1595,7 +1997,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="8">
         <v>7.4</v>
@@ -1603,7 +2005,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="8">
         <v>14.2</v>
@@ -1611,7 +2013,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="8">
         <v>6200</v>
@@ -1619,7 +2021,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="8">
         <v>82</v>
@@ -1672,13 +2074,13 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Daily profit in all documents is now correct
</commit_message>
<xml_diff>
--- a/OptimalBuildingLevel.xlsx
+++ b/OptimalBuildingLevel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BFR-OB-ST-RE" sheetId="4" r:id="rId1"/>
@@ -590,44 +590,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>200512</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>190574</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4962525" y="7239000"/>
-          <a:ext cx="3486637" cy="533474"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
       <xdr:colOff>828675</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
@@ -646,7 +608,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1174,8 +1136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1738,7 +1700,7 @@
   <dimension ref="A2:F42"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2011,7 +1973,7 @@
         <v>25</v>
       </c>
       <c r="B38" s="27">
-        <f>(B32-B20-(B31*(1-B34)/170+1)*B21/(1+B33))*B31*B17*24</f>
+        <f>(B32-B20-(B31*(1-B34)/170+1)*B21/(1+B33))*B31*B28*B17*24</f>
         <v>284645.41533393686</v>
       </c>
     </row>
@@ -2029,7 +1991,7 @@
         <v>45</v>
       </c>
       <c r="B42" s="27">
-        <f>(B32-B20-((B41*(1-B34)/170+1)*B21/(1+B33)))*B41*B17*24</f>
+        <f>(B32-B20-((B41*(1-B34)/170+1)*B21/(1+B33)))*B41*B28*B17*24</f>
         <v>297880.41185193369</v>
       </c>
     </row>
@@ -2045,7 +2007,7 @@
   <dimension ref="A2:F42"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2315,7 +2277,7 @@
         <v>25</v>
       </c>
       <c r="B38" s="27">
-        <f>(B32-B20-(B31*(1-B34)/170+1)*B21/(1+B33))*B31*B17*24</f>
+        <f>(B32-B20-(B31*(1-B34)/170+1)*B21/(1+B33))*B31*B28*B17*24</f>
         <v>289177.06425339356</v>
       </c>
     </row>
@@ -2333,7 +2295,7 @@
         <v>45</v>
       </c>
       <c r="B42" s="27">
-        <f>(B32-B20-((B41*(1-B34)/170+1)*B21/(1+B33)))*B41*B17*24</f>
+        <f>(B32-B20-((B41*(1-B34)/170+1)*B21/(1+B33)))*B41*B28*B17*24</f>
         <v>292771.00753430964</v>
       </c>
     </row>
@@ -2348,8 +2310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M42"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2652,7 +2614,7 @@
         <v>9.0909090909090917</v>
       </c>
       <c r="C24" s="20">
-        <f>C16/C17</f>
+        <f>8/C17</f>
         <v>4.3478260869565215</v>
       </c>
       <c r="D24" s="20">
@@ -2729,19 +2691,19 @@
       </c>
       <c r="B26" s="51">
         <f>B25*$B$41</f>
-        <v>35.623679236006481</v>
+        <v>66.864612730536209</v>
       </c>
       <c r="C26" s="52">
         <f t="shared" ref="C26:L26" si="1">C25*$B$41</f>
-        <v>17.037411808524837</v>
+        <v>31.978727827647752</v>
       </c>
       <c r="D26" s="52">
         <f t="shared" si="1"/>
-        <v>6.9975084213584147</v>
+        <v>13.134120357783896</v>
       </c>
       <c r="E26" s="52">
         <f t="shared" si="1"/>
-        <v>17.037411808524837</v>
+        <v>31.978727827647752</v>
       </c>
       <c r="F26" s="52">
         <f t="shared" si="1"/>
@@ -2795,7 +2757,7 @@
         <v>18</v>
       </c>
       <c r="B31" s="3">
-        <v>39</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -2803,7 +2765,7 @@
         <v>17</v>
       </c>
       <c r="B32" s="6">
-        <v>49000</v>
+        <v>53000</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2819,7 +2781,7 @@
         <v>42</v>
       </c>
       <c r="B34" s="25">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2828,7 +2790,7 @@
       </c>
       <c r="B35" s="17">
         <f>B38/24/B28/B31</f>
-        <v>4899.5397285067929</v>
+        <v>637.7076289592768</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -2837,7 +2799,7 @@
       </c>
       <c r="B36" s="65">
         <f>B32-B35</f>
-        <v>44100.460271493204</v>
+        <v>52362.292371040727</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2846,7 +2808,7 @@
       </c>
       <c r="B37" s="18">
         <f>B36-B21-B20</f>
-        <v>1254.340271493209</v>
+        <v>9516.1723710407314</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2854,8 +2816,8 @@
         <v>25</v>
       </c>
       <c r="B38" s="27">
-        <f>(B32-B20-(B31*(1-B34)/170+1)*B21/(1+B33))*B31*B28*24</f>
-        <v>2130085.9399266057</v>
+        <f>(B32-B20-(B31*(1-B34)/170+1)*B21/(1+B33))*B31*B17*B28*24</f>
+        <v>924149.43001463811</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2864,7 +2826,7 @@
       </c>
       <c r="B41" s="43">
         <f>((B32-B20)*(1+B33)/B21-1)*170/2/(1-B34)</f>
-        <v>76.696011274414559</v>
+        <v>143.9561887436156</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2872,8 +2834,8 @@
         <v>45</v>
       </c>
       <c r="B42" s="27">
-        <f>(B32-B20-((B41*(1-B34)/170+1)*B21/(1+B33)))*B41*B28*24</f>
-        <v>2808551.1409290237</v>
+        <f>(B32-B20-((B41*(1-B34)/170+1)*B21/(1+B33)))*B41*B17*B28*24</f>
+        <v>932917.74906358926</v>
       </c>
     </row>
   </sheetData>

</xml_diff>